<commit_message>
Integrate client tonnage data: auto-derive weight tier per destination
- Add read_tonnage() to parse Tonnage sheet from Freight.xlsx (40HC only)
- Match 37/70 freight destinations to client-provided weight limits
- Default to 23 MT for 33 unmatched destinations
- Remove manual weight dropdown; auto-derive tier via MATCH approximate
- Add 3-layer warning system for unconfirmed tonnage:
  * B11 displays "(UNCONFIRMED)" with red conditional formatting
  * Row 13 red warning banner when using default weight
  * Amber tint on result cells (FOB, Units, Total) when unconfirmed
- Add FR_GrossWT and FR_Confirmed named ranges (24 total)
- Print tonnage data quality report during build (misspellings, duplicates, etc.)
- Update test suite: 9 tests, all passing

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Quotation_Tool.xlsx
+++ b/Quotation_Tool.xlsx
@@ -28,6 +28,8 @@
     <definedName name="FR_Transit">Freight!$E$2:$E$141</definedName>
     <definedName name="FR_USD">Freight!$F$2:$F$141</definedName>
     <definedName name="FR_EUR">Freight!$G$2:$G$141</definedName>
+    <definedName name="FR_GrossWT">Freight!$H$2:$H$141</definedName>
+    <definedName name="FR_Confirmed">Freight!$I$2:$I$141</definedName>
     <definedName name="SizeList">Lists!$A$2:$A$55</definedName>
     <definedName name="ChipsList">Lists!$B$2:$B$12</definedName>
     <definedName name="ECList">Lists!$C$2:$C$6</definedName>
@@ -46,7 +48,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,6 +79,11 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <i val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
@@ -99,7 +106,7 @@
       <sz val="9"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -116,6 +123,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00D6E4F0"/>
         <bgColor rgb="00D6E4F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E0E0E0"/>
+        <bgColor rgb="00E0E0E0"/>
       </patternFill>
     </fill>
     <fill>
@@ -157,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -168,10 +181,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -190,29 +207,63 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="00FFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00CC0000"/>
+          <bgColor rgb="00CC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="00CC0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFC7CE"/>
+          <bgColor rgb="00FFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFF2CC"/>
+          <bgColor rgb="00FFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -630,7 +681,7 @@
       </c>
       <c r="B5" s="5" t="n"/>
       <c r="K5">
-        <f>IFERROR(MATCH(B11,WeightTiers,0),0)</f>
+        <f>IFERROR(MATCH(K11,WeightTiers,1),0)</f>
         <v/>
       </c>
     </row>
@@ -642,7 +693,7 @@
       </c>
       <c r="B6" s="5" t="n"/>
       <c r="K6">
-        <f>AND(B4&lt;&gt;"",B5&lt;&gt;"",B6&lt;&gt;"",B7&lt;&gt;"",B8&lt;&gt;"",B9&lt;&gt;"",B10&lt;&gt;"",B11&lt;&gt;"")</f>
+        <f>AND(B4&lt;&gt;"",B5&lt;&gt;"",B6&lt;&gt;"",B7&lt;&gt;"",B8&lt;&gt;"",B9&lt;&gt;"",B10&lt;&gt;"")</f>
         <v/>
       </c>
     </row>
@@ -700,7 +751,14 @@
           <t>Container Gross Weight (MT)</t>
         </is>
       </c>
-      <c r="B11" s="5" t="n"/>
+      <c r="B11" s="6">
+        <f>IF(B10="","",IF(K5=0,"N/A",INDEX(WeightTiers,K5)&amp;" MT"&amp;IF(K12=0," (UNCONFIRMED)","")))</f>
+        <v/>
+      </c>
+      <c r="K11">
+        <f>IF(K9&gt;0,INDEX(FR_GrossWT,K9),IF(K10&gt;0,INDEX(FR_GrossWT,K10),0))</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
@@ -708,8 +766,18 @@
           <t>EUR / USD Exchange Rate</t>
         </is>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="7" t="n">
         <v>1.08</v>
+      </c>
+      <c r="K12">
+        <f>IF(K9&gt;0,INDEX(FR_Confirmed,K9),IF(K10&gt;0,INDEX(FR_Confirmed,K10),0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <f>IF(AND(B10&lt;&gt;"",K12=0),"WARNING: No confirmed weight data for this destination. Using default 23 MT. Verify before quoting.","")</f>
+        <v/>
       </c>
     </row>
     <row r="14" ht="8" customHeight="1"/>
@@ -728,157 +796,183 @@
       <c r="H15" s="3" t="n"/>
     </row>
     <row r="16" ht="32" customHeight="1">
-      <c r="A16" s="7" t="inlineStr">
+      <c r="A16" s="9" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="B16" s="7" t="inlineStr">
+      <c r="B16" s="9" t="inlineStr">
         <is>
           <t>Product Code</t>
         </is>
       </c>
-      <c r="C16" s="7" t="inlineStr">
+      <c r="C16" s="9" t="inlineStr">
         <is>
           <t>FOB Price / Unit ($)</t>
         </is>
       </c>
-      <c r="D16" s="7" t="inlineStr">
+      <c r="D16" s="9" t="inlineStr">
         <is>
           <t>Freight / Container ($)</t>
         </is>
       </c>
-      <c r="E16" s="7" t="inlineStr">
+      <c r="E16" s="9" t="inlineStr">
         <is>
           <t>Units / Container</t>
         </is>
       </c>
-      <c r="F16" s="7" t="inlineStr">
+      <c r="F16" s="9" t="inlineStr">
         <is>
           <t>Freight / Unit ($)</t>
         </is>
       </c>
-      <c r="G16" s="7" t="inlineStr">
+      <c r="G16" s="9" t="inlineStr">
         <is>
           <t>Total Cost / Unit ($)</t>
         </is>
       </c>
-      <c r="H16" s="7" t="inlineStr">
+      <c r="H16" s="9" t="inlineStr">
         <is>
           <t>Transit Time (Days)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>India</t>
         </is>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11">
         <f>IF(NOT($K$6),"",IF(K7=0,"-",INDEX(IN_ProdNos,K7)))</f>
         <v/>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="12">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_FOB,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="12">
         <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_USD,K9)+INDEX(FR_EUR,K9)*$B$12))</f>
         <v/>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="13">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_PCS,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="14">
         <f>IF(NOT($K$6),"",IFERROR(D17/E17,"-"))</f>
         <v/>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="14">
         <f>IF(NOT($K$6),"",IFERROR(C17+F17,"-"))</f>
         <v/>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="15">
         <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_Transit,K9)))</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="14" t="inlineStr">
+      <c r="A18" s="16" t="inlineStr">
         <is>
           <t>Sri Lanka</t>
         </is>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="17">
         <f>IF(NOT($K$6),"",IF(K8=0,"-",INDEX(SL_ProdNos,K8)))</f>
         <v/>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="18">
         <f>IF(NOT($K$6),"",IF(OR(K8=0,$K$5=0),"-",INDEX(SL_FOB,K8,$K$5)))</f>
         <v/>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="18">
         <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_USD,K10)+INDEX(FR_EUR,K10)*$B$12))</f>
         <v/>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="19">
         <f>IF(NOT($K$6),"",IF(OR(K8=0,$K$5=0),"-",INDEX(SL_PCS,K8,$K$5)))</f>
         <v/>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="20">
         <f>IF(NOT($K$6),"",IFERROR(D18/E18,"-"))</f>
         <v/>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="20">
         <f>IF(NOT($K$6),"",IFERROR(C18+F18,"-"))</f>
         <v/>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="21">
         <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_Transit,K10)))</f>
         <v/>
       </c>
     </row>
     <row r="19" ht="8" customHeight="1"/>
     <row r="20">
-      <c r="A20" s="20">
+      <c r="A20" s="22">
         <f>IF(NOT(K6),"Please fill in all input fields above.",IF(AND(K7=0,K8=0),"No results found with the query inputs.",IF(AND(K7&gt;0,K8&gt;0,K9&gt;0,K10&gt;0),"",IF(AND(K7=0,K8&gt;0),"Product not available from India.",IF(AND(K7&gt;0,K8=0),"Product not available from Sri Lanka.",IF(AND(K9=0,K10&gt;0),"No freight route available from India to this destination.",IF(AND(K9&gt;0,K10=0),"No freight route available from Sri Lanka to this destination.",IF(AND(K9=0,K10=0),"No freight routes available to this destination.",""))))))))</f>
         <v/>
       </c>
     </row>
     <row r="21" ht="8" customHeight="1"/>
     <row r="22">
-      <c r="A22" s="21" t="inlineStr">
+      <c r="A22" s="23" t="inlineStr">
         <is>
           <t>India - Full Description</t>
         </is>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="24">
         <f>IF(NOT(K6),"",IF(K7=0,"-",INDEX(IN_Descs,K7)))</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="21" t="inlineStr">
+      <c r="A23" s="23" t="inlineStr">
         <is>
           <t>Sri Lanka - Full Description</t>
         </is>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="24">
         <f>IF(NOT(K6),"",IF(K8=0,"-",INDEX(SL_Descs,K8)))</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A13:H13"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="B23:H23"/>
   </mergeCells>
-  <dataValidations count="8">
+  <conditionalFormatting sqref="A13:H13">
+    <cfRule type="expression" priority="1" dxfId="0">
+      <formula>AND($B$10&lt;&gt;"",$K$12=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="expression" priority="2" dxfId="1">
+      <formula>AND($B$10&lt;&gt;"",$K$12=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:C18">
+    <cfRule type="expression" priority="3" dxfId="2">
+      <formula>AND($B$10&lt;&gt;"",$K$12=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:E18">
+    <cfRule type="expression" priority="4" dxfId="2">
+      <formula>AND($B$10&lt;&gt;"",$K$12=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G18">
+    <cfRule type="expression" priority="5" dxfId="2">
+      <formula>AND($B$10&lt;&gt;"",$K$12=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="7">
     <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Input" error="Please select a value from the dropdown list." promptTitle="GB Size" prompt="Select GB Size" type="list">
       <formula1>=SizeList</formula1>
     </dataValidation>
@@ -899,9 +993,6 @@
     </dataValidation>
     <dataValidation sqref="B10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Input" error="Please select a value from the dropdown list." promptTitle="Port of Destination" prompt="Select Port of Destination" type="list">
       <formula1>=DestList</formula1>
-    </dataValidation>
-    <dataValidation sqref="B11" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Input" error="Please select a value from the dropdown list." promptTitle="Container Gross Weight (MT)" prompt="Select Container Gross Weight (MT)" type="list">
-      <formula1>=WeightTiers</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -31186,7 +31277,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31230,6 +31321,16 @@
           <t>Total_EUR</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Gross_Weight_MT</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Weight_Confirmed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -31261,6 +31362,12 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
+      <c r="H2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -31292,6 +31399,12 @@
       <c r="G3" t="n">
         <v>0</v>
       </c>
+      <c r="H3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -31323,6 +31436,12 @@
       <c r="G4" t="n">
         <v>0</v>
       </c>
+      <c r="H4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -31354,6 +31473,12 @@
       <c r="G5" t="n">
         <v>346</v>
       </c>
+      <c r="H5" t="n">
+        <v>24</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -31385,6 +31510,12 @@
       <c r="G6" t="n">
         <v>401</v>
       </c>
+      <c r="H6" t="n">
+        <v>24</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -31416,6 +31547,12 @@
       <c r="G7" t="n">
         <v>0</v>
       </c>
+      <c r="H7" t="n">
+        <v>23</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -31447,6 +31584,12 @@
       <c r="G8" t="n">
         <v>0</v>
       </c>
+      <c r="H8" t="n">
+        <v>23</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -31478,6 +31621,12 @@
       <c r="G9" t="n">
         <v>0</v>
       </c>
+      <c r="H9" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -31509,6 +31658,12 @@
       <c r="G10" t="n">
         <v>0</v>
       </c>
+      <c r="H10" t="n">
+        <v>23</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -31523,7 +31678,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Cochin, IN</t>
+          <t>Tuticorin, IN</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -31532,14 +31687,20 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" t="n">
-        <v>599</v>
+        <v>914</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
+      <c r="H11" t="n">
+        <v>23</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -31571,6 +31732,12 @@
       <c r="G12" t="n">
         <v>346</v>
       </c>
+      <c r="H12" t="n">
+        <v>24</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -31602,6 +31769,12 @@
       <c r="G13" t="n">
         <v>0</v>
       </c>
+      <c r="H13" t="n">
+        <v>23</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -31633,6 +31806,12 @@
       <c r="G14" t="n">
         <v>401</v>
       </c>
+      <c r="H14" t="n">
+        <v>24</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -31664,6 +31843,12 @@
       <c r="G15" t="n">
         <v>0</v>
       </c>
+      <c r="H15" t="n">
+        <v>25</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -31695,6 +31880,12 @@
       <c r="G16" t="n">
         <v>275</v>
       </c>
+      <c r="H16" t="n">
+        <v>24</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -31726,6 +31917,12 @@
       <c r="G17" t="n">
         <v>0</v>
       </c>
+      <c r="H17" t="n">
+        <v>22</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -31757,6 +31954,12 @@
       <c r="G18" t="n">
         <v>310</v>
       </c>
+      <c r="H18" t="n">
+        <v>23</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -31788,6 +31991,12 @@
       <c r="G19" t="n">
         <v>0</v>
       </c>
+      <c r="H19" t="n">
+        <v>25</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -31819,6 +32028,12 @@
       <c r="G20" t="n">
         <v>0</v>
       </c>
+      <c r="H20" t="n">
+        <v>23</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -31850,6 +32065,12 @@
       <c r="G21" t="n">
         <v>0</v>
       </c>
+      <c r="H21" t="n">
+        <v>27</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -31881,6 +32102,12 @@
       <c r="G22" t="n">
         <v>0</v>
       </c>
+      <c r="H22" t="n">
+        <v>23</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -31912,6 +32139,12 @@
       <c r="G23" t="n">
         <v>0</v>
       </c>
+      <c r="H23" t="n">
+        <v>23</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -31943,6 +32176,12 @@
       <c r="G24" t="n">
         <v>207</v>
       </c>
+      <c r="H24" t="n">
+        <v>23</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -31974,6 +32213,12 @@
       <c r="G25" t="n">
         <v>0</v>
       </c>
+      <c r="H25" t="n">
+        <v>26</v>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -32005,6 +32250,12 @@
       <c r="G26" t="n">
         <v>0</v>
       </c>
+      <c r="H26" t="n">
+        <v>23</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -32036,6 +32287,12 @@
       <c r="G27" t="n">
         <v>310</v>
       </c>
+      <c r="H27" t="n">
+        <v>23</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -32067,6 +32324,12 @@
       <c r="G28" t="n">
         <v>401</v>
       </c>
+      <c r="H28" t="n">
+        <v>23</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -32098,6 +32361,12 @@
       <c r="G29" t="n">
         <v>0</v>
       </c>
+      <c r="H29" t="n">
+        <v>23</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -32129,6 +32398,12 @@
       <c r="G30" t="n">
         <v>0</v>
       </c>
+      <c r="H30" t="n">
+        <v>25</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -32160,6 +32435,12 @@
       <c r="G31" t="n">
         <v>0</v>
       </c>
+      <c r="H31" t="n">
+        <v>23</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -32191,6 +32472,12 @@
       <c r="G32" t="n">
         <v>0</v>
       </c>
+      <c r="H32" t="n">
+        <v>20</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -32222,6 +32509,12 @@
       <c r="G33" t="n">
         <v>0</v>
       </c>
+      <c r="H33" t="n">
+        <v>22</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -32253,6 +32546,12 @@
       <c r="G34" t="n">
         <v>0</v>
       </c>
+      <c r="H34" t="n">
+        <v>23</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -32284,6 +32583,12 @@
       <c r="G35" t="n">
         <v>0</v>
       </c>
+      <c r="H35" t="n">
+        <v>23</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -32315,6 +32620,12 @@
       <c r="G36" t="n">
         <v>310</v>
       </c>
+      <c r="H36" t="n">
+        <v>23</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -32346,6 +32657,12 @@
       <c r="G37" t="n">
         <v>0</v>
       </c>
+      <c r="H37" t="n">
+        <v>23</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -32377,6 +32694,12 @@
       <c r="G38" t="n">
         <v>401</v>
       </c>
+      <c r="H38" t="n">
+        <v>24</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -32408,6 +32731,12 @@
       <c r="G39" t="n">
         <v>310</v>
       </c>
+      <c r="H39" t="n">
+        <v>23</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -32439,6 +32768,12 @@
       <c r="G40" t="n">
         <v>260</v>
       </c>
+      <c r="H40" t="n">
+        <v>25</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -32470,6 +32805,12 @@
       <c r="G41" t="n">
         <v>260</v>
       </c>
+      <c r="H41" t="n">
+        <v>25</v>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -32501,6 +32842,12 @@
       <c r="G42" t="n">
         <v>0</v>
       </c>
+      <c r="H42" t="n">
+        <v>23</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -32532,6 +32879,12 @@
       <c r="G43" t="n">
         <v>0</v>
       </c>
+      <c r="H43" t="n">
+        <v>26</v>
+      </c>
+      <c r="I43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -32563,6 +32916,12 @@
       <c r="G44" t="n">
         <v>0</v>
       </c>
+      <c r="H44" t="n">
+        <v>23</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -32594,6 +32953,12 @@
       <c r="G45" t="n">
         <v>401</v>
       </c>
+      <c r="H45" t="n">
+        <v>23</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -32625,6 +32990,12 @@
       <c r="G46" t="n">
         <v>0</v>
       </c>
+      <c r="H46" t="n">
+        <v>25</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -32656,6 +33027,12 @@
       <c r="G47" t="n">
         <v>0</v>
       </c>
+      <c r="H47" t="n">
+        <v>25</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -32687,6 +33064,12 @@
       <c r="G48" t="n">
         <v>0</v>
       </c>
+      <c r="H48" t="n">
+        <v>25</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -32718,6 +33101,12 @@
       <c r="G49" t="n">
         <v>0</v>
       </c>
+      <c r="H49" t="n">
+        <v>23</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -32749,6 +33138,12 @@
       <c r="G50" t="n">
         <v>310</v>
       </c>
+      <c r="H50" t="n">
+        <v>23</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -32780,6 +33175,12 @@
       <c r="G51" t="n">
         <v>0</v>
       </c>
+      <c r="H51" t="n">
+        <v>26</v>
+      </c>
+      <c r="I51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -32811,6 +33212,12 @@
       <c r="G52" t="n">
         <v>0</v>
       </c>
+      <c r="H52" t="n">
+        <v>23</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -32842,6 +33249,12 @@
       <c r="G53" t="n">
         <v>418</v>
       </c>
+      <c r="H53" t="n">
+        <v>25</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -32873,6 +33286,12 @@
       <c r="G54" t="n">
         <v>0</v>
       </c>
+      <c r="H54" t="n">
+        <v>23</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -32904,6 +33323,12 @@
       <c r="G55" t="n">
         <v>0</v>
       </c>
+      <c r="H55" t="n">
+        <v>23</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -32935,6 +33360,12 @@
       <c r="G56" t="n">
         <v>0</v>
       </c>
+      <c r="H56" t="n">
+        <v>27</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -32966,6 +33397,12 @@
       <c r="G57" t="n">
         <v>310</v>
       </c>
+      <c r="H57" t="n">
+        <v>23</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -32997,6 +33434,12 @@
       <c r="G58" t="n">
         <v>0</v>
       </c>
+      <c r="H58" t="n">
+        <v>23</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -33028,6 +33471,12 @@
       <c r="G59" t="n">
         <v>0</v>
       </c>
+      <c r="H59" t="n">
+        <v>26</v>
+      </c>
+      <c r="I59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -33059,6 +33508,12 @@
       <c r="G60" t="n">
         <v>0</v>
       </c>
+      <c r="H60" t="n">
+        <v>25</v>
+      </c>
+      <c r="I60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -33090,6 +33545,12 @@
       <c r="G61" t="n">
         <v>0</v>
       </c>
+      <c r="H61" t="n">
+        <v>25</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -33121,6 +33582,12 @@
       <c r="G62" t="n">
         <v>630</v>
       </c>
+      <c r="H62" t="n">
+        <v>23</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -33152,6 +33619,12 @@
       <c r="G63" t="n">
         <v>0</v>
       </c>
+      <c r="H63" t="n">
+        <v>22</v>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -33183,6 +33656,12 @@
       <c r="G64" t="n">
         <v>401</v>
       </c>
+      <c r="H64" t="n">
+        <v>24</v>
+      </c>
+      <c r="I64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -33214,6 +33693,12 @@
       <c r="G65" t="n">
         <v>0</v>
       </c>
+      <c r="H65" t="n">
+        <v>23</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -33245,6 +33730,12 @@
       <c r="G66" t="n">
         <v>0</v>
       </c>
+      <c r="H66" t="n">
+        <v>23</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -33276,6 +33767,12 @@
       <c r="G67" t="n">
         <v>346</v>
       </c>
+      <c r="H67" t="n">
+        <v>24</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -33307,6 +33804,12 @@
       <c r="G68" t="n">
         <v>0</v>
       </c>
+      <c r="H68" t="n">
+        <v>23</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -33338,6 +33841,12 @@
       <c r="G69" t="n">
         <v>310</v>
       </c>
+      <c r="H69" t="n">
+        <v>23</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -33369,6 +33878,12 @@
       <c r="G70" t="n">
         <v>0</v>
       </c>
+      <c r="H70" t="n">
+        <v>23</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -33400,6 +33915,12 @@
       <c r="G71" t="n">
         <v>0</v>
       </c>
+      <c r="H71" t="n">
+        <v>26</v>
+      </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -33431,6 +33952,12 @@
       <c r="G72" t="n">
         <v>0</v>
       </c>
+      <c r="H72" t="n">
+        <v>23</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -33462,6 +33989,12 @@
       <c r="G73" t="n">
         <v>0</v>
       </c>
+      <c r="H73" t="n">
+        <v>27</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -33493,6 +34026,12 @@
       <c r="G74" t="n">
         <v>0</v>
       </c>
+      <c r="H74" t="n">
+        <v>25</v>
+      </c>
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -33524,6 +34063,12 @@
       <c r="G75" t="n">
         <v>346</v>
       </c>
+      <c r="H75" t="n">
+        <v>24</v>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -33555,6 +34100,12 @@
       <c r="G76" t="n">
         <v>401</v>
       </c>
+      <c r="H76" t="n">
+        <v>24</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -33586,6 +34137,12 @@
       <c r="G77" t="n">
         <v>0</v>
       </c>
+      <c r="H77" t="n">
+        <v>23</v>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -33617,6 +34174,12 @@
       <c r="G78" t="n">
         <v>0</v>
       </c>
+      <c r="H78" t="n">
+        <v>23</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -33648,6 +34211,12 @@
       <c r="G79" t="n">
         <v>0</v>
       </c>
+      <c r="H79" t="n">
+        <v>25</v>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -33679,6 +34248,12 @@
       <c r="G80" t="n">
         <v>0</v>
       </c>
+      <c r="H80" t="n">
+        <v>23</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -33710,6 +34285,12 @@
       <c r="G81" t="n">
         <v>0</v>
       </c>
+      <c r="H81" t="n">
+        <v>23</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -33741,6 +34322,12 @@
       <c r="G82" t="n">
         <v>346</v>
       </c>
+      <c r="H82" t="n">
+        <v>24</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -33772,6 +34359,12 @@
       <c r="G83" t="n">
         <v>0</v>
       </c>
+      <c r="H83" t="n">
+        <v>23</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -33803,6 +34396,12 @@
       <c r="G84" t="n">
         <v>401</v>
       </c>
+      <c r="H84" t="n">
+        <v>24</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -33834,6 +34433,12 @@
       <c r="G85" t="n">
         <v>0</v>
       </c>
+      <c r="H85" t="n">
+        <v>25</v>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -33865,6 +34470,12 @@
       <c r="G86" t="n">
         <v>275</v>
       </c>
+      <c r="H86" t="n">
+        <v>24</v>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -33896,6 +34507,12 @@
       <c r="G87" t="n">
         <v>0</v>
       </c>
+      <c r="H87" t="n">
+        <v>22</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -33927,6 +34544,12 @@
       <c r="G88" t="n">
         <v>310</v>
       </c>
+      <c r="H88" t="n">
+        <v>23</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -33958,6 +34581,12 @@
       <c r="G89" t="n">
         <v>0</v>
       </c>
+      <c r="H89" t="n">
+        <v>25</v>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -33989,6 +34618,12 @@
       <c r="G90" t="n">
         <v>0</v>
       </c>
+      <c r="H90" t="n">
+        <v>23</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -34020,6 +34655,12 @@
       <c r="G91" t="n">
         <v>0</v>
       </c>
+      <c r="H91" t="n">
+        <v>27</v>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -34051,6 +34692,12 @@
       <c r="G92" t="n">
         <v>0</v>
       </c>
+      <c r="H92" t="n">
+        <v>23</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -34082,6 +34729,12 @@
       <c r="G93" t="n">
         <v>0</v>
       </c>
+      <c r="H93" t="n">
+        <v>23</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -34113,6 +34766,12 @@
       <c r="G94" t="n">
         <v>207</v>
       </c>
+      <c r="H94" t="n">
+        <v>23</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -34144,6 +34803,12 @@
       <c r="G95" t="n">
         <v>0</v>
       </c>
+      <c r="H95" t="n">
+        <v>26</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -34175,6 +34840,12 @@
       <c r="G96" t="n">
         <v>0</v>
       </c>
+      <c r="H96" t="n">
+        <v>23</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -34206,6 +34877,12 @@
       <c r="G97" t="n">
         <v>310</v>
       </c>
+      <c r="H97" t="n">
+        <v>23</v>
+      </c>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -34237,6 +34914,12 @@
       <c r="G98" t="n">
         <v>401</v>
       </c>
+      <c r="H98" t="n">
+        <v>23</v>
+      </c>
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -34268,6 +34951,12 @@
       <c r="G99" t="n">
         <v>0</v>
       </c>
+      <c r="H99" t="n">
+        <v>23</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -34299,6 +34988,12 @@
       <c r="G100" t="n">
         <v>0</v>
       </c>
+      <c r="H100" t="n">
+        <v>25</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -34330,6 +35025,12 @@
       <c r="G101" t="n">
         <v>0</v>
       </c>
+      <c r="H101" t="n">
+        <v>23</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -34361,6 +35062,12 @@
       <c r="G102" t="n">
         <v>0</v>
       </c>
+      <c r="H102" t="n">
+        <v>20</v>
+      </c>
+      <c r="I102" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -34392,6 +35099,12 @@
       <c r="G103" t="n">
         <v>0</v>
       </c>
+      <c r="H103" t="n">
+        <v>22</v>
+      </c>
+      <c r="I103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -34423,6 +35136,12 @@
       <c r="G104" t="n">
         <v>0</v>
       </c>
+      <c r="H104" t="n">
+        <v>23</v>
+      </c>
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -34454,6 +35173,12 @@
       <c r="G105" t="n">
         <v>0</v>
       </c>
+      <c r="H105" t="n">
+        <v>23</v>
+      </c>
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -34485,6 +35210,12 @@
       <c r="G106" t="n">
         <v>310</v>
       </c>
+      <c r="H106" t="n">
+        <v>23</v>
+      </c>
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -34516,6 +35247,12 @@
       <c r="G107" t="n">
         <v>0</v>
       </c>
+      <c r="H107" t="n">
+        <v>23</v>
+      </c>
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -34547,6 +35284,12 @@
       <c r="G108" t="n">
         <v>401</v>
       </c>
+      <c r="H108" t="n">
+        <v>24</v>
+      </c>
+      <c r="I108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -34578,6 +35321,12 @@
       <c r="G109" t="n">
         <v>310</v>
       </c>
+      <c r="H109" t="n">
+        <v>23</v>
+      </c>
+      <c r="I109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -34609,6 +35358,12 @@
       <c r="G110" t="n">
         <v>260</v>
       </c>
+      <c r="H110" t="n">
+        <v>25</v>
+      </c>
+      <c r="I110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -34640,6 +35395,12 @@
       <c r="G111" t="n">
         <v>260</v>
       </c>
+      <c r="H111" t="n">
+        <v>25</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -34671,6 +35432,12 @@
       <c r="G112" t="n">
         <v>0</v>
       </c>
+      <c r="H112" t="n">
+        <v>23</v>
+      </c>
+      <c r="I112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -34702,6 +35469,12 @@
       <c r="G113" t="n">
         <v>0</v>
       </c>
+      <c r="H113" t="n">
+        <v>26</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -34733,6 +35506,12 @@
       <c r="G114" t="n">
         <v>0</v>
       </c>
+      <c r="H114" t="n">
+        <v>23</v>
+      </c>
+      <c r="I114" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -34764,6 +35543,12 @@
       <c r="G115" t="n">
         <v>401</v>
       </c>
+      <c r="H115" t="n">
+        <v>23</v>
+      </c>
+      <c r="I115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -34795,6 +35580,12 @@
       <c r="G116" t="n">
         <v>0</v>
       </c>
+      <c r="H116" t="n">
+        <v>25</v>
+      </c>
+      <c r="I116" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -34826,6 +35617,12 @@
       <c r="G117" t="n">
         <v>0</v>
       </c>
+      <c r="H117" t="n">
+        <v>25</v>
+      </c>
+      <c r="I117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -34857,6 +35654,12 @@
       <c r="G118" t="n">
         <v>0</v>
       </c>
+      <c r="H118" t="n">
+        <v>25</v>
+      </c>
+      <c r="I118" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -34888,6 +35691,12 @@
       <c r="G119" t="n">
         <v>0</v>
       </c>
+      <c r="H119" t="n">
+        <v>23</v>
+      </c>
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -34919,6 +35728,12 @@
       <c r="G120" t="n">
         <v>310</v>
       </c>
+      <c r="H120" t="n">
+        <v>23</v>
+      </c>
+      <c r="I120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -34950,6 +35765,12 @@
       <c r="G121" t="n">
         <v>0</v>
       </c>
+      <c r="H121" t="n">
+        <v>26</v>
+      </c>
+      <c r="I121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -34981,6 +35802,12 @@
       <c r="G122" t="n">
         <v>0</v>
       </c>
+      <c r="H122" t="n">
+        <v>23</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -35012,6 +35839,12 @@
       <c r="G123" t="n">
         <v>418</v>
       </c>
+      <c r="H123" t="n">
+        <v>25</v>
+      </c>
+      <c r="I123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -35043,6 +35876,12 @@
       <c r="G124" t="n">
         <v>0</v>
       </c>
+      <c r="H124" t="n">
+        <v>23</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -35074,6 +35913,12 @@
       <c r="G125" t="n">
         <v>0</v>
       </c>
+      <c r="H125" t="n">
+        <v>23</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -35105,6 +35950,12 @@
       <c r="G126" t="n">
         <v>0</v>
       </c>
+      <c r="H126" t="n">
+        <v>27</v>
+      </c>
+      <c r="I126" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -35136,6 +35987,12 @@
       <c r="G127" t="n">
         <v>310</v>
       </c>
+      <c r="H127" t="n">
+        <v>23</v>
+      </c>
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -35167,6 +36024,12 @@
       <c r="G128" t="n">
         <v>0</v>
       </c>
+      <c r="H128" t="n">
+        <v>23</v>
+      </c>
+      <c r="I128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -35198,6 +36061,12 @@
       <c r="G129" t="n">
         <v>0</v>
       </c>
+      <c r="H129" t="n">
+        <v>26</v>
+      </c>
+      <c r="I129" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -35229,6 +36098,12 @@
       <c r="G130" t="n">
         <v>0</v>
       </c>
+      <c r="H130" t="n">
+        <v>25</v>
+      </c>
+      <c r="I130" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -35260,6 +36135,12 @@
       <c r="G131" t="n">
         <v>0</v>
       </c>
+      <c r="H131" t="n">
+        <v>25</v>
+      </c>
+      <c r="I131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -35291,6 +36172,12 @@
       <c r="G132" t="n">
         <v>630</v>
       </c>
+      <c r="H132" t="n">
+        <v>23</v>
+      </c>
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -35322,6 +36209,12 @@
       <c r="G133" t="n">
         <v>0</v>
       </c>
+      <c r="H133" t="n">
+        <v>22</v>
+      </c>
+      <c r="I133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -35353,6 +36246,12 @@
       <c r="G134" t="n">
         <v>401</v>
       </c>
+      <c r="H134" t="n">
+        <v>24</v>
+      </c>
+      <c r="I134" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -35384,6 +36283,12 @@
       <c r="G135" t="n">
         <v>0</v>
       </c>
+      <c r="H135" t="n">
+        <v>23</v>
+      </c>
+      <c r="I135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -35415,6 +36320,12 @@
       <c r="G136" t="n">
         <v>0</v>
       </c>
+      <c r="H136" t="n">
+        <v>23</v>
+      </c>
+      <c r="I136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -35446,6 +36357,12 @@
       <c r="G137" t="n">
         <v>346</v>
       </c>
+      <c r="H137" t="n">
+        <v>24</v>
+      </c>
+      <c r="I137" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -35477,6 +36394,12 @@
       <c r="G138" t="n">
         <v>0</v>
       </c>
+      <c r="H138" t="n">
+        <v>23</v>
+      </c>
+      <c r="I138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -35508,6 +36431,12 @@
       <c r="G139" t="n">
         <v>310</v>
       </c>
+      <c r="H139" t="n">
+        <v>23</v>
+      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -35539,6 +36468,12 @@
       <c r="G140" t="n">
         <v>0</v>
       </c>
+      <c r="H140" t="n">
+        <v>23</v>
+      </c>
+      <c r="I140" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -35569,6 +36504,12 @@
       </c>
       <c r="G141" t="n">
         <v>0</v>
+      </c>
+      <c r="H141" t="n">
+        <v>26</v>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply 1.0605 multiplier (1% insurance + 5% margin) to freight totals
The client's multiplier is now applied to the sum of all charge codes
per route, not just the base rate. Hardcoded in the Freight/Container
formula as (USD + EUR * rate) * 1.0605.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Quotation_Tool.xlsx
+++ b/Quotation_Tool.xlsx
@@ -852,7 +852,7 @@
         <v/>
       </c>
       <c r="D17" s="12">
-        <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_USD,K9)+INDEX(FR_EUR,K9)*$B$12))</f>
+        <f>IF(NOT($K$6),"",IF(K9=0,"-",(INDEX(FR_USD,K9)+INDEX(FR_EUR,K9)*$B$12)*1.0605))</f>
         <v/>
       </c>
       <c r="E17" s="13">
@@ -887,7 +887,7 @@
         <v/>
       </c>
       <c r="D18" s="18">
-        <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_USD,K10)+INDEX(FR_EUR,K10)*$B$12))</f>
+        <f>IF(NOT($K$6),"",IF(K10=0,"-",(INDEX(FR_USD,K10)+INDEX(FR_EUR,K10)*$B$12)*1.0605))</f>
         <v/>
       </c>
       <c r="E18" s="19">

</xml_diff>

<commit_message>
Use BAS (base ocean freight) only for freight cost, not sum of all charges
Client confirmed the 1.0605 multiplier applies to BAS only, not the
total of all surcharges. Freight/Container formula is now:
  BAS_USD * 1.0605

BAS is extracted separately during freight parsing and stored in
column J (FR_BAS named range). Total USD/EUR columns retained for
reference.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Quotation_Tool.xlsx
+++ b/Quotation_Tool.xlsx
@@ -30,6 +30,7 @@
     <definedName name="FR_EUR">Freight!$G$2:$G$141</definedName>
     <definedName name="FR_GrossWT">Freight!$H$2:$H$141</definedName>
     <definedName name="FR_Confirmed">Freight!$I$2:$I$141</definedName>
+    <definedName name="FR_BAS">Freight!$J$2:$J$141</definedName>
     <definedName name="SizeList">Lists!$A$2:$A$55</definedName>
     <definedName name="ChipsList">Lists!$B$2:$B$12</definedName>
     <definedName name="ECList">Lists!$C$2:$C$6</definedName>
@@ -852,7 +853,7 @@
         <v/>
       </c>
       <c r="D17" s="12">
-        <f>IF(NOT($K$6),"",IF(K9=0,"-",(INDEX(FR_USD,K9)+INDEX(FR_EUR,K9)*$B$12)*1.0605))</f>
+        <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_BAS,K9)*1.0605))</f>
         <v/>
       </c>
       <c r="E17" s="13">
@@ -887,7 +888,7 @@
         <v/>
       </c>
       <c r="D18" s="18">
-        <f>IF(NOT($K$6),"",IF(K10=0,"-",(INDEX(FR_USD,K10)+INDEX(FR_EUR,K10)*$B$12)*1.0605))</f>
+        <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_BAS,K10)*1.0605))</f>
         <v/>
       </c>
       <c r="E18" s="19">
@@ -31277,7 +31278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31331,6 +31332,11 @@
           <t>Weight_Confirmed</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>BAS_USD</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -31368,6 +31374,9 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
+      <c r="J2" t="n">
+        <v>2400</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -31405,6 +31414,9 @@
       <c r="I3" t="n">
         <v>1</v>
       </c>
+      <c r="J3" t="n">
+        <v>2122</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -31442,6 +31454,9 @@
       <c r="I4" t="n">
         <v>1</v>
       </c>
+      <c r="J4" t="n">
+        <v>1140</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -31479,6 +31494,9 @@
       <c r="I5" t="n">
         <v>1</v>
       </c>
+      <c r="J5" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -31516,6 +31534,9 @@
       <c r="I6" t="n">
         <v>1</v>
       </c>
+      <c r="J6" t="n">
+        <v>1290</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -31553,6 +31574,9 @@
       <c r="I7" t="n">
         <v>1</v>
       </c>
+      <c r="J7" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -31590,6 +31614,9 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
+      <c r="J8" t="n">
+        <v>3250</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -31627,6 +31654,9 @@
       <c r="I9" t="n">
         <v>1</v>
       </c>
+      <c r="J9" t="n">
+        <v>890</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -31664,6 +31694,9 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
+      <c r="J10" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -31701,6 +31734,9 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
+      <c r="J11" t="n">
+        <v>830</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -31738,6 +31774,9 @@
       <c r="I12" t="n">
         <v>1</v>
       </c>
+      <c r="J12" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -31775,6 +31814,9 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
+      <c r="J13" t="n">
+        <v>1490</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -31812,6 +31854,9 @@
       <c r="I14" t="n">
         <v>1</v>
       </c>
+      <c r="J14" t="n">
+        <v>1340</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -31849,6 +31894,9 @@
       <c r="I15" t="n">
         <v>1</v>
       </c>
+      <c r="J15" t="n">
+        <v>2425</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -31886,6 +31934,9 @@
       <c r="I16" t="n">
         <v>1</v>
       </c>
+      <c r="J16" t="n">
+        <v>1519</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -31923,6 +31974,9 @@
       <c r="I17" t="n">
         <v>1</v>
       </c>
+      <c r="J17" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -31960,6 +32014,9 @@
       <c r="I18" t="n">
         <v>0</v>
       </c>
+      <c r="J18" t="n">
+        <v>1530</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -31997,6 +32054,9 @@
       <c r="I19" t="n">
         <v>1</v>
       </c>
+      <c r="J19" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -32034,6 +32094,9 @@
       <c r="I20" t="n">
         <v>0</v>
       </c>
+      <c r="J20" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -32071,6 +32134,9 @@
       <c r="I21" t="n">
         <v>1</v>
       </c>
+      <c r="J21" t="n">
+        <v>1290</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -32108,6 +32174,9 @@
       <c r="I22" t="n">
         <v>0</v>
       </c>
+      <c r="J22" t="n">
+        <v>1400</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -32145,6 +32214,9 @@
       <c r="I23" t="n">
         <v>0</v>
       </c>
+      <c r="J23" t="n">
+        <v>1750</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -32182,6 +32254,9 @@
       <c r="I24" t="n">
         <v>0</v>
       </c>
+      <c r="J24" t="n">
+        <v>1960</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -32219,6 +32294,9 @@
       <c r="I25" t="n">
         <v>1</v>
       </c>
+      <c r="J25" t="n">
+        <v>670</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -32256,6 +32334,9 @@
       <c r="I26" t="n">
         <v>0</v>
       </c>
+      <c r="J26" t="n">
+        <v>2350</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -32293,6 +32374,9 @@
       <c r="I27" t="n">
         <v>0</v>
       </c>
+      <c r="J27" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -32330,6 +32414,9 @@
       <c r="I28" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="n">
+        <v>1490</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -32367,6 +32454,9 @@
       <c r="I29" t="n">
         <v>0</v>
       </c>
+      <c r="J29" t="n">
+        <v>1290</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -32404,6 +32494,9 @@
       <c r="I30" t="n">
         <v>1</v>
       </c>
+      <c r="J30" t="n">
+        <v>1550</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -32441,6 +32534,9 @@
       <c r="I31" t="n">
         <v>0</v>
       </c>
+      <c r="J31" t="n">
+        <v>1190</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -32478,6 +32574,9 @@
       <c r="I32" t="n">
         <v>1</v>
       </c>
+      <c r="J32" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -32515,6 +32614,9 @@
       <c r="I33" t="n">
         <v>1</v>
       </c>
+      <c r="J33" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -32552,6 +32654,9 @@
       <c r="I34" t="n">
         <v>0</v>
       </c>
+      <c r="J34" t="n">
+        <v>2693</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -32589,6 +32694,9 @@
       <c r="I35" t="n">
         <v>0</v>
       </c>
+      <c r="J35" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -32626,6 +32734,9 @@
       <c r="I36" t="n">
         <v>0</v>
       </c>
+      <c r="J36" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -32663,6 +32774,9 @@
       <c r="I37" t="n">
         <v>0</v>
       </c>
+      <c r="J37" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -32700,6 +32814,9 @@
       <c r="I38" t="n">
         <v>1</v>
       </c>
+      <c r="J38" t="n">
+        <v>1820</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -32737,6 +32854,9 @@
       <c r="I39" t="n">
         <v>0</v>
       </c>
+      <c r="J39" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -32774,6 +32894,9 @@
       <c r="I40" t="n">
         <v>1</v>
       </c>
+      <c r="J40" t="n">
+        <v>1510</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -32811,6 +32934,9 @@
       <c r="I41" t="n">
         <v>1</v>
       </c>
+      <c r="J41" t="n">
+        <v>990</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -32848,6 +32974,9 @@
       <c r="I42" t="n">
         <v>0</v>
       </c>
+      <c r="J42" t="n">
+        <v>1850</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -32885,6 +33014,9 @@
       <c r="I43" t="n">
         <v>1</v>
       </c>
+      <c r="J43" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -32922,6 +33054,9 @@
       <c r="I44" t="n">
         <v>1</v>
       </c>
+      <c r="J44" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -32959,6 +33094,9 @@
       <c r="I45" t="n">
         <v>0</v>
       </c>
+      <c r="J45" t="n">
+        <v>1290</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -32996,6 +33134,9 @@
       <c r="I46" t="n">
         <v>1</v>
       </c>
+      <c r="J46" t="n">
+        <v>2350</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -33033,6 +33174,9 @@
       <c r="I47" t="n">
         <v>1</v>
       </c>
+      <c r="J47" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -33070,6 +33214,9 @@
       <c r="I48" t="n">
         <v>1</v>
       </c>
+      <c r="J48" t="n">
+        <v>1400</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -33107,6 +33254,9 @@
       <c r="I49" t="n">
         <v>0</v>
       </c>
+      <c r="J49" t="n">
+        <v>2850</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -33144,6 +33294,9 @@
       <c r="I50" t="n">
         <v>0</v>
       </c>
+      <c r="J50" t="n">
+        <v>890</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -33181,6 +33334,9 @@
       <c r="I51" t="n">
         <v>1</v>
       </c>
+      <c r="J51" t="n">
+        <v>348</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -33218,6 +33374,9 @@
       <c r="I52" t="n">
         <v>0</v>
       </c>
+      <c r="J52" t="n">
+        <v>2250</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -33255,6 +33414,9 @@
       <c r="I53" t="n">
         <v>1</v>
       </c>
+      <c r="J53" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -33292,6 +33454,9 @@
       <c r="I54" t="n">
         <v>0</v>
       </c>
+      <c r="J54" t="n">
+        <v>1770</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -33329,6 +33494,9 @@
       <c r="I55" t="n">
         <v>0</v>
       </c>
+      <c r="J55" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -33366,6 +33534,9 @@
       <c r="I56" t="n">
         <v>1</v>
       </c>
+      <c r="J56" t="n">
+        <v>1490</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -33403,6 +33574,9 @@
       <c r="I57" t="n">
         <v>0</v>
       </c>
+      <c r="J57" t="n">
+        <v>1090</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -33440,6 +33614,9 @@
       <c r="I58" t="n">
         <v>0</v>
       </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -33477,6 +33654,9 @@
       <c r="I59" t="n">
         <v>1</v>
       </c>
+      <c r="J59" t="n">
+        <v>1540</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -33514,6 +33694,9 @@
       <c r="I60" t="n">
         <v>1</v>
       </c>
+      <c r="J60" t="n">
+        <v>2250</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -33551,6 +33734,9 @@
       <c r="I61" t="n">
         <v>1</v>
       </c>
+      <c r="J61" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -33588,6 +33774,9 @@
       <c r="I62" t="n">
         <v>0</v>
       </c>
+      <c r="J62" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -33625,6 +33814,9 @@
       <c r="I63" t="n">
         <v>1</v>
       </c>
+      <c r="J63" t="n">
+        <v>3050</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -33662,6 +33854,9 @@
       <c r="I64" t="n">
         <v>1</v>
       </c>
+      <c r="J64" t="n">
+        <v>1953</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -33699,6 +33894,9 @@
       <c r="I65" t="n">
         <v>1</v>
       </c>
+      <c r="J65" t="n">
+        <v>2700</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -33736,6 +33934,9 @@
       <c r="I66" t="n">
         <v>0</v>
       </c>
+      <c r="J66" t="n">
+        <v>3790</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -33773,6 +33974,9 @@
       <c r="I67" t="n">
         <v>1</v>
       </c>
+      <c r="J67" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -33810,6 +34014,9 @@
       <c r="I68" t="n">
         <v>0</v>
       </c>
+      <c r="J68" t="n">
+        <v>1950</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -33847,6 +34054,9 @@
       <c r="I69" t="n">
         <v>0</v>
       </c>
+      <c r="J69" t="n">
+        <v>790</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -33884,6 +34094,9 @@
       <c r="I70" t="n">
         <v>1</v>
       </c>
+      <c r="J70" t="n">
+        <v>1450</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -33921,6 +34134,9 @@
       <c r="I71" t="n">
         <v>1</v>
       </c>
+      <c r="J71" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -33958,6 +34174,9 @@
       <c r="I72" t="n">
         <v>0</v>
       </c>
+      <c r="J72" t="n">
+        <v>2250</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -33995,6 +34214,9 @@
       <c r="I73" t="n">
         <v>1</v>
       </c>
+      <c r="J73" t="n">
+        <v>1972</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -34032,6 +34254,9 @@
       <c r="I74" t="n">
         <v>1</v>
       </c>
+      <c r="J74" t="n">
+        <v>990</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -34069,6 +34294,9 @@
       <c r="I75" t="n">
         <v>1</v>
       </c>
+      <c r="J75" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -34106,6 +34334,9 @@
       <c r="I76" t="n">
         <v>1</v>
       </c>
+      <c r="J76" t="n">
+        <v>1140</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -34143,6 +34374,9 @@
       <c r="I77" t="n">
         <v>1</v>
       </c>
+      <c r="J77" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -34180,6 +34414,9 @@
       <c r="I78" t="n">
         <v>0</v>
       </c>
+      <c r="J78" t="n">
+        <v>3100</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -34217,6 +34454,9 @@
       <c r="I79" t="n">
         <v>1</v>
       </c>
+      <c r="J79" t="n">
+        <v>740</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -34254,6 +34494,9 @@
       <c r="I80" t="n">
         <v>0</v>
       </c>
+      <c r="J80" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -34291,6 +34534,9 @@
       <c r="I81" t="n">
         <v>0</v>
       </c>
+      <c r="J81" t="n">
+        <v>550</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -34328,6 +34574,9 @@
       <c r="I82" t="n">
         <v>1</v>
       </c>
+      <c r="J82" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -34365,6 +34614,9 @@
       <c r="I83" t="n">
         <v>0</v>
       </c>
+      <c r="J83" t="n">
+        <v>1340</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -34402,6 +34654,9 @@
       <c r="I84" t="n">
         <v>1</v>
       </c>
+      <c r="J84" t="n">
+        <v>1190</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -34439,6 +34694,9 @@
       <c r="I85" t="n">
         <v>1</v>
       </c>
+      <c r="J85" t="n">
+        <v>2275</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -34476,6 +34734,9 @@
       <c r="I86" t="n">
         <v>1</v>
       </c>
+      <c r="J86" t="n">
+        <v>1369</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -34513,6 +34774,9 @@
       <c r="I87" t="n">
         <v>1</v>
       </c>
+      <c r="J87" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -34550,6 +34814,9 @@
       <c r="I88" t="n">
         <v>0</v>
       </c>
+      <c r="J88" t="n">
+        <v>1380</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -34587,6 +34854,9 @@
       <c r="I89" t="n">
         <v>1</v>
       </c>
+      <c r="J89" t="n">
+        <v>1350</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -34624,6 +34894,9 @@
       <c r="I90" t="n">
         <v>0</v>
       </c>
+      <c r="J90" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -34661,6 +34934,9 @@
       <c r="I91" t="n">
         <v>1</v>
       </c>
+      <c r="J91" t="n">
+        <v>1140</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -34698,6 +34974,9 @@
       <c r="I92" t="n">
         <v>0</v>
       </c>
+      <c r="J92" t="n">
+        <v>1250</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -34735,6 +35014,9 @@
       <c r="I93" t="n">
         <v>0</v>
       </c>
+      <c r="J93" t="n">
+        <v>1600</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -34772,6 +35054,9 @@
       <c r="I94" t="n">
         <v>0</v>
       </c>
+      <c r="J94" t="n">
+        <v>1810</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -34809,6 +35094,9 @@
       <c r="I95" t="n">
         <v>1</v>
       </c>
+      <c r="J95" t="n">
+        <v>1020</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -34846,6 +35134,9 @@
       <c r="I96" t="n">
         <v>0</v>
       </c>
+      <c r="J96" t="n">
+        <v>2200</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -34883,6 +35174,9 @@
       <c r="I97" t="n">
         <v>0</v>
       </c>
+      <c r="J97" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -34920,6 +35214,9 @@
       <c r="I98" t="n">
         <v>0</v>
       </c>
+      <c r="J98" t="n">
+        <v>1340</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -34957,6 +35254,9 @@
       <c r="I99" t="n">
         <v>0</v>
       </c>
+      <c r="J99" t="n">
+        <v>1140</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -34994,6 +35294,9 @@
       <c r="I100" t="n">
         <v>1</v>
       </c>
+      <c r="J100" t="n">
+        <v>1400</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -35031,6 +35334,9 @@
       <c r="I101" t="n">
         <v>0</v>
       </c>
+      <c r="J101" t="n">
+        <v>1040</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -35068,6 +35374,9 @@
       <c r="I102" t="n">
         <v>1</v>
       </c>
+      <c r="J102" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -35105,6 +35414,9 @@
       <c r="I103" t="n">
         <v>1</v>
       </c>
+      <c r="J103" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -35142,6 +35454,9 @@
       <c r="I104" t="n">
         <v>0</v>
       </c>
+      <c r="J104" t="n">
+        <v>2543</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -35179,6 +35494,9 @@
       <c r="I105" t="n">
         <v>0</v>
       </c>
+      <c r="J105" t="n">
+        <v>353</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -35216,6 +35534,9 @@
       <c r="I106" t="n">
         <v>0</v>
       </c>
+      <c r="J106" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -35253,6 +35574,9 @@
       <c r="I107" t="n">
         <v>0</v>
       </c>
+      <c r="J107" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -35290,6 +35614,9 @@
       <c r="I108" t="n">
         <v>1</v>
       </c>
+      <c r="J108" t="n">
+        <v>1670</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -35327,6 +35654,9 @@
       <c r="I109" t="n">
         <v>0</v>
       </c>
+      <c r="J109" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -35364,6 +35694,9 @@
       <c r="I110" t="n">
         <v>1</v>
       </c>
+      <c r="J110" t="n">
+        <v>1360</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -35401,6 +35734,9 @@
       <c r="I111" t="n">
         <v>1</v>
       </c>
+      <c r="J111" t="n">
+        <v>840</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -35438,6 +35774,9 @@
       <c r="I112" t="n">
         <v>0</v>
       </c>
+      <c r="J112" t="n">
+        <v>1700</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -35475,6 +35814,9 @@
       <c r="I113" t="n">
         <v>1</v>
       </c>
+      <c r="J113" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -35512,6 +35854,9 @@
       <c r="I114" t="n">
         <v>1</v>
       </c>
+      <c r="J114" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -35549,6 +35894,9 @@
       <c r="I115" t="n">
         <v>0</v>
       </c>
+      <c r="J115" t="n">
+        <v>1140</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -35586,6 +35934,9 @@
       <c r="I116" t="n">
         <v>1</v>
       </c>
+      <c r="J116" t="n">
+        <v>2200</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -35623,6 +35974,9 @@
       <c r="I117" t="n">
         <v>1</v>
       </c>
+      <c r="J117" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -35660,6 +36014,9 @@
       <c r="I118" t="n">
         <v>1</v>
       </c>
+      <c r="J118" t="n">
+        <v>1250</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -35697,6 +36054,9 @@
       <c r="I119" t="n">
         <v>0</v>
       </c>
+      <c r="J119" t="n">
+        <v>2700</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -35734,6 +36094,9 @@
       <c r="I120" t="n">
         <v>0</v>
       </c>
+      <c r="J120" t="n">
+        <v>740</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -35771,6 +36134,9 @@
       <c r="I121" t="n">
         <v>1</v>
       </c>
+      <c r="J121" t="n">
+        <v>571</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -35808,6 +36174,9 @@
       <c r="I122" t="n">
         <v>0</v>
       </c>
+      <c r="J122" t="n">
+        <v>2100</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -35845,6 +36214,9 @@
       <c r="I123" t="n">
         <v>1</v>
       </c>
+      <c r="J123" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -35882,6 +36254,9 @@
       <c r="I124" t="n">
         <v>0</v>
       </c>
+      <c r="J124" t="n">
+        <v>2120</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -35919,6 +36294,9 @@
       <c r="I125" t="n">
         <v>0</v>
       </c>
+      <c r="J125" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -35956,6 +36334,9 @@
       <c r="I126" t="n">
         <v>1</v>
       </c>
+      <c r="J126" t="n">
+        <v>1340</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -35993,6 +36374,9 @@
       <c r="I127" t="n">
         <v>0</v>
       </c>
+      <c r="J127" t="n">
+        <v>940</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -36030,6 +36414,9 @@
       <c r="I128" t="n">
         <v>0</v>
       </c>
+      <c r="J128" t="n">
+        <v>420</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -36067,6 +36454,9 @@
       <c r="I129" t="n">
         <v>1</v>
       </c>
+      <c r="J129" t="n">
+        <v>1390</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -36104,6 +36494,9 @@
       <c r="I130" t="n">
         <v>1</v>
       </c>
+      <c r="J130" t="n">
+        <v>2100</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -36141,6 +36534,9 @@
       <c r="I131" t="n">
         <v>1</v>
       </c>
+      <c r="J131" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -36178,6 +36574,9 @@
       <c r="I132" t="n">
         <v>0</v>
       </c>
+      <c r="J132" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -36215,6 +36614,9 @@
       <c r="I133" t="n">
         <v>1</v>
       </c>
+      <c r="J133" t="n">
+        <v>2900</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -36252,6 +36654,9 @@
       <c r="I134" t="n">
         <v>1</v>
       </c>
+      <c r="J134" t="n">
+        <v>1803</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -36289,6 +36694,9 @@
       <c r="I135" t="n">
         <v>1</v>
       </c>
+      <c r="J135" t="n">
+        <v>2550</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -36326,6 +36734,9 @@
       <c r="I136" t="n">
         <v>0</v>
       </c>
+      <c r="J136" t="n">
+        <v>3640</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -36363,6 +36774,9 @@
       <c r="I137" t="n">
         <v>1</v>
       </c>
+      <c r="J137" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -36400,6 +36814,9 @@
       <c r="I138" t="n">
         <v>0</v>
       </c>
+      <c r="J138" t="n">
+        <v>1800</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -36437,6 +36854,9 @@
       <c r="I139" t="n">
         <v>0</v>
       </c>
+      <c r="J139" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -36474,6 +36894,9 @@
       <c r="I140" t="n">
         <v>1</v>
       </c>
+      <c r="J140" t="n">
+        <v>1300</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -36510,6 +36933,9 @@
       </c>
       <c r="I141" t="n">
         <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add discount column: editable B12 input (default 30%), Disc. FOB in results
Total cost now uses discounted FOB + freight/unit. Result rows expanded
to 9 columns (A-I). Tests updated with discount arithmetic verification.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Quotation_Tool.xlsx
+++ b/Quotation_Tool.xlsx
@@ -169,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -181,6 +181,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -633,11 +636,11 @@
     <col width="24" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="5" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
     <col hidden="1" width="22" customWidth="1" min="11" max="11"/>
   </cols>
@@ -757,13 +760,21 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Discount (%)</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>0.3</v>
+      </c>
       <c r="K12">
         <f>IF(K9&gt;0,INDEX(FR_GrossWT,K9),IF(K10&gt;0,INDEX(FR_GrossWT,K10),IF(K11&gt;0,INDEX(FR_GrossWT,K11),0)))</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7">
+      <c r="A13" s="8">
         <f>IF(AND(B10&lt;&gt;"",K13=0),"WARNING: No confirmed weight data for this destination. Using default 23 MT. Verify before quoting.","")</f>
         <v/>
       </c>
@@ -786,195 +797,213 @@
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
+      <c r="I15" s="3" t="n"/>
     </row>
     <row r="16" ht="32" customHeight="1">
-      <c r="A16" s="8" t="inlineStr">
+      <c r="A16" s="9" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="B16" s="8" t="inlineStr">
+      <c r="B16" s="9" t="inlineStr">
         <is>
           <t>Product Code</t>
         </is>
       </c>
-      <c r="C16" s="8" t="inlineStr">
+      <c r="C16" s="9" t="inlineStr">
         <is>
           <t>FOB Price / Unit ($)</t>
         </is>
       </c>
-      <c r="D16" s="8" t="inlineStr">
+      <c r="D16" s="9" t="inlineStr">
+        <is>
+          <t>Disc. FOB / Unit ($)</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
         <is>
           <t>Freight / Container ($)</t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+      <c r="F16" s="9" t="inlineStr">
         <is>
           <t>Units / Container</t>
         </is>
       </c>
-      <c r="F16" s="8" t="inlineStr">
+      <c r="G16" s="9" t="inlineStr">
         <is>
           <t>Freight / Unit ($)</t>
         </is>
       </c>
-      <c r="G16" s="8" t="inlineStr">
+      <c r="H16" s="9" t="inlineStr">
         <is>
           <t>Total Cost / Unit ($)</t>
         </is>
       </c>
-      <c r="H16" s="8" t="inlineStr">
+      <c r="I16" s="9" t="inlineStr">
         <is>
           <t>Transit Time (Days)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="inlineStr">
+      <c r="A17" s="10" t="inlineStr">
         <is>
           <t>Cochin, IN</t>
         </is>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <f>IF(NOT($K$6),"",IF(K7=0,"-",INDEX(IN_ProdNos,K7)))</f>
         <v/>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="12">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_FOB,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
+        <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",C17*(1-$B$12)))</f>
+        <v/>
+      </c>
+      <c r="E17" s="12">
         <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_AllIn,K9)*1.0605))</f>
         <v/>
       </c>
-      <c r="E17" s="12">
+      <c r="F17" s="13">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_PCS,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="F17" s="13">
-        <f>IF(NOT($K$6),"",IFERROR(D17/E17,"-"))</f>
+      <c r="G17" s="14">
+        <f>IF(NOT($K$6),"",IFERROR(E17/F17,"-"))</f>
         <v/>
       </c>
-      <c r="G17" s="13">
-        <f>IF(NOT($K$6),"",IFERROR(C17+F17,"-"))</f>
+      <c r="H17" s="14">
+        <f>IF(NOT($K$6),"",IFERROR(D17+G17,"-"))</f>
         <v/>
       </c>
-      <c r="H17" s="14">
+      <c r="I17" s="15">
         <f>IF(NOT($K$6),"",IF(K9=0,"-",INDEX(FR_Transit,K9)))</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="inlineStr">
+      <c r="A18" s="16" t="inlineStr">
         <is>
           <t>Tuticorin, IN</t>
         </is>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="17">
         <f>IF(NOT($K$6),"",IF(K7=0,"-",INDEX(IN_ProdNos,K7)))</f>
         <v/>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="18">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_FOB,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="18">
+        <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",C18*(1-$B$12)))</f>
+        <v/>
+      </c>
+      <c r="E18" s="18">
         <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_AllIn,K10)*1.0605))</f>
         <v/>
       </c>
-      <c r="E18" s="18">
+      <c r="F18" s="19">
         <f>IF(NOT($K$6),"",IF(OR(K7=0,$K$5=0),"-",INDEX(IN_PCS,K7,$K$5)))</f>
         <v/>
       </c>
-      <c r="F18" s="19">
-        <f>IF(NOT($K$6),"",IFERROR(D18/E18,"-"))</f>
+      <c r="G18" s="20">
+        <f>IF(NOT($K$6),"",IFERROR(E18/F18,"-"))</f>
         <v/>
       </c>
-      <c r="G18" s="19">
-        <f>IF(NOT($K$6),"",IFERROR(C18+F18,"-"))</f>
+      <c r="H18" s="20">
+        <f>IF(NOT($K$6),"",IFERROR(D18+G18,"-"))</f>
         <v/>
       </c>
-      <c r="H18" s="20">
+      <c r="I18" s="21">
         <f>IF(NOT($K$6),"",IF(K10=0,"-",INDEX(FR_Transit,K10)))</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="inlineStr">
+      <c r="A19" s="10" t="inlineStr">
         <is>
           <t>Colombo, LK</t>
         </is>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="11">
         <f>IF(NOT($K$6),"",IF(K8=0,"-",INDEX(SL_ProdNos,K8)))</f>
         <v/>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="12">
         <f>IF(NOT($K$6),"",IF(OR(K8=0,$K$5=0),"-",INDEX(SL_FOB,K8,$K$5)))</f>
         <v/>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="12">
+        <f>IF(NOT($K$6),"",IF(OR(K8=0,$K$5=0),"-",C19*(1-$B$12)))</f>
+        <v/>
+      </c>
+      <c r="E19" s="12">
         <f>IF(NOT($K$6),"",IF(K11=0,"-",INDEX(FR_AllIn,K11)*1.0605))</f>
         <v/>
       </c>
-      <c r="E19" s="12">
+      <c r="F19" s="13">
         <f>IF(NOT($K$6),"",IF(OR(K8=0,$K$5=0),"-",INDEX(SL_PCS,K8,$K$5)))</f>
         <v/>
       </c>
-      <c r="F19" s="13">
-        <f>IF(NOT($K$6),"",IFERROR(D19/E19,"-"))</f>
+      <c r="G19" s="14">
+        <f>IF(NOT($K$6),"",IFERROR(E19/F19,"-"))</f>
         <v/>
       </c>
-      <c r="G19" s="13">
-        <f>IF(NOT($K$6),"",IFERROR(C19+F19,"-"))</f>
+      <c r="H19" s="14">
+        <f>IF(NOT($K$6),"",IFERROR(D19+G19,"-"))</f>
         <v/>
       </c>
-      <c r="H19" s="14">
+      <c r="I19" s="15">
         <f>IF(NOT($K$6),"",IF(K11=0,"-",INDEX(FR_Transit,K11)))</f>
         <v/>
       </c>
     </row>
     <row r="20" ht="8" customHeight="1"/>
     <row r="21">
-      <c r="A21" s="21">
+      <c r="A21" s="22">
         <f>IF(NOT(K6),"Please fill in all input fields above.",IF(AND(K7=0,K8=0),"No results found with the query inputs.",IF(AND(K7&gt;0,K8&gt;0,K9&gt;0,K10&gt;0,K11&gt;0),"",IF(AND(K7=0,K8&gt;0),"Product not available from India.",IF(AND(K7&gt;0,K8=0),"Product not available from Sri Lanka.",IF(AND(K9=0,K10=0,K11&gt;0),"No freight routes available from India to this destination.",IF(AND(K9&gt;0,K10&gt;0,K11=0),"No freight route available from Sri Lanka to this destination.",IF(AND(K9=0,K10=0,K11=0),"No freight routes available to this destination.",""))))))))</f>
         <v/>
       </c>
     </row>
     <row r="22" ht="8" customHeight="1"/>
     <row r="23">
-      <c r="A23" s="22" t="inlineStr">
+      <c r="A23" s="23" t="inlineStr">
         <is>
           <t>India - Full Description</t>
         </is>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="24">
         <f>IF(NOT(K6),"",IF(K7=0,"-",INDEX(IN_Descs,K7)))</f>
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="22" t="inlineStr">
+      <c r="A24" s="23" t="inlineStr">
         <is>
           <t>Sri Lanka - Full Description</t>
         </is>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="24">
         <f>IF(NOT(K6),"",IF(K8=0,"-",INDEX(SL_Descs,K8)))</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B23:I23"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A21:I21"/>
   </mergeCells>
-  <conditionalFormatting sqref="A13:H13">
+  <conditionalFormatting sqref="A13:I13">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>AND($B$10&lt;&gt;"",$K$13=0)</formula>
     </cfRule>
@@ -989,13 +1018,18 @@
       <formula>AND($B$10&lt;&gt;"",$K$13=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E19">
+  <conditionalFormatting sqref="D17:D19">
     <cfRule type="expression" priority="4" dxfId="2">
       <formula>AND($B$10&lt;&gt;"",$K$13=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G19">
+  <conditionalFormatting sqref="F17:F19">
     <cfRule type="expression" priority="5" dxfId="2">
+      <formula>AND($B$10&lt;&gt;"",$K$13=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:H19">
+    <cfRule type="expression" priority="6" dxfId="2">
       <formula>AND($B$10&lt;&gt;"",$K$13=0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Soften warning colors from red to orange tone
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Quotation_Tool.xlsx
+++ b/Quotation_Tool.xlsx
@@ -237,20 +237,20 @@
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00CC0000"/>
-          <bgColor rgb="00CC0000"/>
+          <fgColor rgb="00E67E22"/>
+          <bgColor rgb="00E67E22"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
         <b val="1"/>
-        <color rgb="00CC0000"/>
+        <color rgb="00E67E22"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFC7CE"/>
-          <bgColor rgb="00FFC7CE"/>
+          <fgColor rgb="00FDEBD0"/>
+          <bgColor rgb="00FDEBD0"/>
         </patternFill>
       </fill>
     </dxf>

</xml_diff>